<commit_message>
fix data format: allow null and change audit datetime to date
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenziping/Desktop/20200918AAB/AABKoala/Local Program/upload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenziping/Desktop/20200918AAB/AABKoala/LocalProgram/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E799D45D-C5FC-C545-94AD-0810A0680EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204AF84-A9A9-3545-BD45-BA11C5B3F2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2740" windowWidth="27840" windowHeight="16940" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
+    <workbookView xWindow="4200" yWindow="2700" windowWidth="27840" windowHeight="16940" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -127,24 +127,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TRP_6</t>
-  </si>
-  <si>
-    <t>TRP_15</t>
-  </si>
-  <si>
-    <t>TRP_18</t>
-  </si>
-  <si>
-    <t>TRP_6FFF</t>
-  </si>
-  <si>
-    <t>TRP_10FFF</t>
-  </si>
-  <si>
-    <t>TRP_10</t>
-  </si>
-  <si>
     <t>Reading_101106</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -445,6 +427,24 @@
   <si>
     <t>Acu</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TPR_6</t>
+  </si>
+  <si>
+    <t>TPR_10</t>
+  </si>
+  <si>
+    <t>TPR_15</t>
+  </si>
+  <si>
+    <t>TPR_18</t>
+  </si>
+  <si>
+    <t>TPR_6FFF</t>
+  </si>
+  <si>
+    <t>TPR_10FFF</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -517,7 +517,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
   <dimension ref="A1:DA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="DB2" sqref="DB2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -934,250 +934,250 @@
         <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AR1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AS1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AT1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AU1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AV1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AW1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AX1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AY1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AZ1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BA1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BB1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BC1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BD1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BE1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BF1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BG1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BH1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BI1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BJ1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BK1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BL1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BM1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BN1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BO1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BP1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BR1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BS1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BT1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BU1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BV1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BQ1" t="s">
+      <c r="BW1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BX1" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BY1" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BZ1" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CA1" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CB1" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CC1" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CD1" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CE1" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CF1" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CG1" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CH1" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CI1" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CJ1" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CK1" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CL1" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CM1" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CN1" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CO1" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CP1" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CQ1" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CR1" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CS1" t="s">
         <v>89</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CT1" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CU1" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CV1" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CW1" t="s">
         <v>93</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CX1" t="s">
         <v>94</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CY1" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CZ1" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DA1" t="s">
         <v>97</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>102</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:105">
@@ -1185,43 +1185,43 @@
         <v>3081</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H2" s="3">
         <v>42648</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="R2">
         <v>1.002</v>

</xml_diff>

<commit_message>
update result request to accommondate IMRT
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenziping/Desktop/20200918AAB/AABKoala/LocalProgram/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27A251-8DB1-EA44-8130-B83F6194DD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CCCB0D-2D77-4846-90CC-65AADD919E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67920" yWindow="15300" windowWidth="38700" windowHeight="22460" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="35840" windowHeight="20600" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andrew Alves</author>
+  </authors>
+  <commentList>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{39147E03-B549-B84D-AE03-0659C44ED793}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andrew Alves:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+formal report not issued</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
   <si>
     <t>Reading_101106</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -389,13 +423,339 @@
   </si>
   <si>
     <t>fac_10FFF</t>
+  </si>
+  <si>
+    <t>c6_p12_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p13_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p14_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p15_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p16_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p17_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p11_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p12_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p13_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p14_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p15_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p16_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p17_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p11_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p12_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p13_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p14_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p15_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p17_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p18_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p11_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p12_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p13_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p14_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p15_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p16_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6_p17_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p11_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p12_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p13_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p14_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p15_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p16_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7_p17_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p11_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p12_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p13_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p14_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p15_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p17_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8_p18_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aardvark</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>Clem</t>
+  </si>
+  <si>
+    <t>TRFF7</t>
+  </si>
+  <si>
+    <t>Roland</t>
+  </si>
+  <si>
+    <t>RAV</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>c6_p11_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p11_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p12_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p13_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p14_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p15_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p16_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p17_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p11_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p12_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p13_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p14_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p15_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p16_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p17_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p11_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p12_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p13_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p14_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p15_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p17_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p18_6</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p11_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p12_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p13_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p14_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p15_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p16_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c6_p17_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p11_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p12_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p13_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p14_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p15_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p16_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c7_p17_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p11_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p12_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p13_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p14_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p15_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p17_10</t>
+  </si>
+  <si>
+    <t>imrt_misdelivery_c8_p18_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,13 +778,45 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -456,7 +848,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -464,11 +856,113 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -788,11 +1282,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
-  <dimension ref="A1:DB1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
+  <dimension ref="A1:GH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="EH1" workbookViewId="0">
+      <selection activeCell="ER1" sqref="ER1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -806,9 +1300,11 @@
     <col min="32" max="32" width="28.6640625" customWidth="1"/>
     <col min="33" max="33" width="32.33203125" customWidth="1"/>
     <col min="68" max="68" width="28.6640625" customWidth="1"/>
+    <col min="190" max="190" width="40.83203125" customWidth="1"/>
+    <col min="191" max="191" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" s="2" customFormat="1">
+    <row r="1" spans="1:190" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -1126,21 +1622,967 @@
       </c>
       <c r="DB1" t="s">
         <v>74</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="DV1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="DW1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DX1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="DY1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="DZ1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="EB1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="ED1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="EE1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="EF1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EH1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="EI1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="EK1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="EL1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="EM1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="EN1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="EP1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="EQ1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="ER1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="ES1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="ET1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="EU1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="EV1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="EW1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="EX1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EY1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="EZ1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="FA1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="FB1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="FC1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="FD1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="FE1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="FF1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="FG1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="FH1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="FI1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="FJ1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="FK1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="FL1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="FM1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="FN1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="FO1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="FP1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="FQ1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="FR1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="FS1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="FT1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="FU1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="FV1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="FW1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="FX1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FY1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FZ1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="GA1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="GB1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GC1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="GD1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="GE1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="GF1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="GG1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="GH1" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:190">
+      <c r="B2" s="3">
+        <v>3001</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6">
+        <v>40963</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="S2" s="7">
+        <v>1</v>
+      </c>
+      <c r="T2" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U2" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V2" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W2" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X2" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="8">
+        <v>-3.1543391443251117E-3</v>
+      </c>
+      <c r="AF2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>6.0371586820287988E-3</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>3.9750517405645711E-2</v>
+      </c>
+      <c r="AI2" s="9">
+        <v>5.1635985501662868E-3</v>
+      </c>
+      <c r="AJ2" s="9">
+        <v>-0.45805634681773166</v>
+      </c>
+      <c r="AK2" s="9">
+        <v>2.3452377767241458E-2</v>
+      </c>
+      <c r="AL2" s="9">
+        <v>6.96269787557625E-2</v>
+      </c>
+      <c r="AM2" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AN2" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO2" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP2" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AR2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AS2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AT2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AU2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AV2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AW2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AX2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AY2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AZ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BA2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BB2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BC2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BD2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BE2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BF2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BG2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BH2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BI2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BJ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BK2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BL2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BM2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BN2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BO2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BP2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
+        <v>0</v>
+      </c>
+      <c r="CG2">
+        <v>0</v>
+      </c>
+      <c r="CH2">
+        <v>0</v>
+      </c>
+      <c r="CI2">
+        <v>0</v>
+      </c>
+      <c r="CJ2">
+        <v>0</v>
+      </c>
+      <c r="CK2">
+        <v>0</v>
+      </c>
+      <c r="CL2">
+        <v>0</v>
+      </c>
+      <c r="CM2">
+        <v>0</v>
+      </c>
+      <c r="CN2">
+        <v>0</v>
+      </c>
+      <c r="CO2">
+        <v>0</v>
+      </c>
+      <c r="CP2">
+        <v>0</v>
+      </c>
+      <c r="CQ2">
+        <v>0</v>
+      </c>
+      <c r="CR2">
+        <v>0</v>
+      </c>
+      <c r="CS2">
+        <v>0</v>
+      </c>
+      <c r="CT2">
+        <v>0</v>
+      </c>
+      <c r="CU2">
+        <v>0</v>
+      </c>
+      <c r="CV2">
+        <v>0</v>
+      </c>
+      <c r="CW2">
+        <v>0</v>
+      </c>
+      <c r="CX2">
+        <v>0</v>
+      </c>
+      <c r="CY2">
+        <v>0</v>
+      </c>
+      <c r="CZ2">
+        <v>0</v>
+      </c>
+      <c r="DA2">
+        <v>0</v>
+      </c>
+      <c r="DB2">
+        <v>0</v>
+      </c>
+      <c r="DC2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DD2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DE2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DF2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DG2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DH2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DI2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DJ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DK2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DL2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DM2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DN2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DO2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DP2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DQ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DR2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DS2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DT2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DU2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DV2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DW2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DX2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DY2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="DZ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EA2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EB2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EC2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="ED2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EE2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EF2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EG2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EH2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EI2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EJ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EK2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EL2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EM2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EN2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EO2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EP2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EQ2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="ER2" s="8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="ES2">
+        <v>0</v>
+      </c>
+      <c r="ET2">
+        <v>0</v>
+      </c>
+      <c r="EU2">
+        <v>0</v>
+      </c>
+      <c r="EV2">
+        <v>0</v>
+      </c>
+      <c r="EW2">
+        <v>0</v>
+      </c>
+      <c r="EX2">
+        <v>0</v>
+      </c>
+      <c r="EY2">
+        <v>0</v>
+      </c>
+      <c r="EZ2">
+        <v>0</v>
+      </c>
+      <c r="FA2">
+        <v>0</v>
+      </c>
+      <c r="FB2">
+        <v>0</v>
+      </c>
+      <c r="FC2">
+        <v>0</v>
+      </c>
+      <c r="FD2">
+        <v>0</v>
+      </c>
+      <c r="FE2">
+        <v>0</v>
+      </c>
+      <c r="FF2">
+        <v>0</v>
+      </c>
+      <c r="FG2">
+        <v>0</v>
+      </c>
+      <c r="FH2">
+        <v>0</v>
+      </c>
+      <c r="FI2">
+        <v>0</v>
+      </c>
+      <c r="FJ2">
+        <v>0</v>
+      </c>
+      <c r="FK2">
+        <v>0</v>
+      </c>
+      <c r="FL2">
+        <v>0</v>
+      </c>
+      <c r="FM2">
+        <v>0</v>
+      </c>
+      <c r="FN2">
+        <v>0</v>
+      </c>
+      <c r="FO2">
+        <v>0</v>
+      </c>
+      <c r="FP2">
+        <v>0</v>
+      </c>
+      <c r="FQ2">
+        <v>0</v>
+      </c>
+      <c r="FR2">
+        <v>0</v>
+      </c>
+      <c r="FS2">
+        <v>0</v>
+      </c>
+      <c r="FT2">
+        <v>0</v>
+      </c>
+      <c r="FU2">
+        <v>0</v>
+      </c>
+      <c r="FV2">
+        <v>0</v>
+      </c>
+      <c r="FW2">
+        <v>0</v>
+      </c>
+      <c r="FX2">
+        <v>0</v>
+      </c>
+      <c r="FY2">
+        <v>0</v>
+      </c>
+      <c r="FZ2">
+        <v>0</v>
+      </c>
+      <c r="GA2">
+        <v>0</v>
+      </c>
+      <c r="GB2">
+        <v>0</v>
+      </c>
+      <c r="GC2">
+        <v>0</v>
+      </c>
+      <c r="GD2">
+        <v>0</v>
+      </c>
+      <c r="GE2">
+        <v>0</v>
+      </c>
+      <c r="GF2">
+        <v>0</v>
+      </c>
+      <c r="GG2">
+        <v>0</v>
+      </c>
+      <c r="GH2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1">
-    <cfRule type="expression" dxfId="1" priority="53">
+    <cfRule type="expression" dxfId="16" priority="68">
       <formula>IF(ISNA(A1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AC1">
-    <cfRule type="expression" dxfId="0" priority="52">
+    <cfRule type="expression" dxfId="15" priority="67">
       <formula>IF(ISNA(X1),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E2">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>IF(ISNA(B2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:J2">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>IF(ISNA(F2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>IF(ISNA(K2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>IF(ISNA(M2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>IF(ISNA(N2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>IF(N2="Monaco",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>IF(N2="Xio",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>IF(N2="Pinnacle",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>IF(N2="Eclipse",TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>IF(ISNA(O2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:Q2">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>IF(ISNA(P2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:X2">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>IF(ISNA(S2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y2:AD2">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF(ISNA(Y2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2:BP2">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF(ISNA(AE2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DC2:ER2">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(ISNA(DC2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix create result list
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenziping/Desktop/20200918AAB/AABKoala/LocalProgram/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CCCB0D-2D77-4846-90CC-65AADD919E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8909EF-08A8-AD4D-8A07-A67D1C09E435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="35840" windowHeight="20600" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
   </bookViews>
@@ -32,42 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andrew Alves</author>
-  </authors>
-  <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{39147E03-B549-B84D-AE03-0659C44ED793}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrew Alves:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-formal report not issued</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Reading_101106</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -587,33 +553,6 @@
   <si>
     <t>c8_p18_10</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aardvark</t>
-  </si>
-  <si>
-    <t>Terry</t>
-  </si>
-  <si>
-    <t>Clem</t>
-  </si>
-  <si>
-    <t>TRFF7</t>
-  </si>
-  <si>
-    <t>Roland</t>
-  </si>
-  <si>
-    <t>RAV</t>
-  </si>
-  <si>
-    <t>Sun</t>
-  </si>
-  <si>
-    <t>Great</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>c6_p11_6</t>
@@ -751,11 +690,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="0.0%"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -778,45 +713,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -848,7 +751,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -856,113 +759,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -1282,11 +1083,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
-  <dimension ref="A1:GH2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
+  <dimension ref="A1:GH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EH1" workbookViewId="0">
-      <selection activeCell="ER1" sqref="ER1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1624,7 +1425,7 @@
         <v>74</v>
       </c>
       <c r="DC1" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="DD1" s="2" t="s">
         <v>106</v>
@@ -1750,839 +1551,145 @@
         <v>146</v>
       </c>
       <c r="ES1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="ET1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="EU1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="EV1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="EW1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="EX1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="EY1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="EZ1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="FA1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="FB1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="ET1" s="2" t="s">
+      <c r="FC1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="EU1" s="2" t="s">
+      <c r="FD1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="EV1" s="2" t="s">
+      <c r="FE1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="EW1" s="2" t="s">
+      <c r="FF1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="EX1" s="2" t="s">
+      <c r="FG1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="EY1" s="2" t="s">
+      <c r="FH1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="EZ1" s="2" t="s">
+      <c r="FI1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="FA1" s="2" t="s">
+      <c r="FJ1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="FB1" s="2" t="s">
+      <c r="FK1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="FC1" s="2" t="s">
+      <c r="FL1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="FD1" s="2" t="s">
+      <c r="FM1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="FE1" s="2" t="s">
+      <c r="FN1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="FF1" s="2" t="s">
+      <c r="FO1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="FG1" s="2" t="s">
+      <c r="FP1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="FH1" s="2" t="s">
+      <c r="FQ1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="FI1" s="2" t="s">
+      <c r="FR1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="FJ1" s="2" t="s">
+      <c r="FS1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="FK1" s="2" t="s">
+      <c r="FT1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="FL1" s="2" t="s">
+      <c r="FU1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="FM1" s="2" t="s">
+      <c r="FV1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="FN1" s="2" t="s">
+      <c r="FW1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="FO1" s="2" t="s">
+      <c r="FX1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="FP1" s="2" t="s">
+      <c r="FY1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="FQ1" s="2" t="s">
+      <c r="FZ1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="FR1" s="2" t="s">
+      <c r="GA1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="FS1" s="2" t="s">
+      <c r="GB1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="FT1" s="2" t="s">
+      <c r="GC1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="FU1" s="2" t="s">
+      <c r="GD1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="FV1" s="2" t="s">
+      <c r="GE1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="FW1" s="2" t="s">
+      <c r="GF1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="FX1" s="2" t="s">
+      <c r="GG1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="FY1" s="2" t="s">
+      <c r="GH1" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="FZ1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="GA1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="GB1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GC1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="GD1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="GE1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="GF1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="GG1" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="GH1" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:190">
-      <c r="B2" s="3">
-        <v>3001</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6">
-        <v>40963</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" t="s">
-        <v>151</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="S2" s="7">
-        <v>1</v>
-      </c>
-      <c r="T2" s="7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U2" s="7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V2" s="7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W2" s="7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X2" s="7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="8">
-        <v>-3.1543391443251117E-3</v>
-      </c>
-      <c r="AF2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG2" s="8">
-        <v>6.0371586820287988E-3</v>
-      </c>
-      <c r="AH2" s="9">
-        <v>3.9750517405645711E-2</v>
-      </c>
-      <c r="AI2" s="9">
-        <v>5.1635985501662868E-3</v>
-      </c>
-      <c r="AJ2" s="9">
-        <v>-0.45805634681773166</v>
-      </c>
-      <c r="AK2" s="9">
-        <v>2.3452377767241458E-2</v>
-      </c>
-      <c r="AL2" s="9">
-        <v>6.96269787557625E-2</v>
-      </c>
-      <c r="AM2" s="9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AN2" s="9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO2" s="9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AP2" s="9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AQ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AR2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AS2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AT2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AU2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AV2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AW2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AX2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AY2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AZ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BA2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BB2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BC2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BD2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BE2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BF2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BG2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BH2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BI2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BJ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BK2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BL2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BM2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BN2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BO2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BP2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="BQ2">
-        <v>0</v>
-      </c>
-      <c r="BR2">
-        <v>0</v>
-      </c>
-      <c r="BS2">
-        <v>0</v>
-      </c>
-      <c r="BT2">
-        <v>0</v>
-      </c>
-      <c r="BU2">
-        <v>0</v>
-      </c>
-      <c r="BV2">
-        <v>0</v>
-      </c>
-      <c r="BW2">
-        <v>0</v>
-      </c>
-      <c r="BX2">
-        <v>0</v>
-      </c>
-      <c r="BY2">
-        <v>0</v>
-      </c>
-      <c r="BZ2">
-        <v>0</v>
-      </c>
-      <c r="CA2">
-        <v>0</v>
-      </c>
-      <c r="CB2">
-        <v>0</v>
-      </c>
-      <c r="CC2">
-        <v>0</v>
-      </c>
-      <c r="CD2">
-        <v>0</v>
-      </c>
-      <c r="CE2">
-        <v>0</v>
-      </c>
-      <c r="CF2">
-        <v>0</v>
-      </c>
-      <c r="CG2">
-        <v>0</v>
-      </c>
-      <c r="CH2">
-        <v>0</v>
-      </c>
-      <c r="CI2">
-        <v>0</v>
-      </c>
-      <c r="CJ2">
-        <v>0</v>
-      </c>
-      <c r="CK2">
-        <v>0</v>
-      </c>
-      <c r="CL2">
-        <v>0</v>
-      </c>
-      <c r="CM2">
-        <v>0</v>
-      </c>
-      <c r="CN2">
-        <v>0</v>
-      </c>
-      <c r="CO2">
-        <v>0</v>
-      </c>
-      <c r="CP2">
-        <v>0</v>
-      </c>
-      <c r="CQ2">
-        <v>0</v>
-      </c>
-      <c r="CR2">
-        <v>0</v>
-      </c>
-      <c r="CS2">
-        <v>0</v>
-      </c>
-      <c r="CT2">
-        <v>0</v>
-      </c>
-      <c r="CU2">
-        <v>0</v>
-      </c>
-      <c r="CV2">
-        <v>0</v>
-      </c>
-      <c r="CW2">
-        <v>0</v>
-      </c>
-      <c r="CX2">
-        <v>0</v>
-      </c>
-      <c r="CY2">
-        <v>0</v>
-      </c>
-      <c r="CZ2">
-        <v>0</v>
-      </c>
-      <c r="DA2">
-        <v>0</v>
-      </c>
-      <c r="DB2">
-        <v>0</v>
-      </c>
-      <c r="DC2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DD2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DE2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DF2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DG2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DH2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DI2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DJ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DK2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DL2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DM2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DN2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DO2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DP2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DQ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DR2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DS2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DT2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DU2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DV2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DW2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DX2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DY2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="DZ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EA2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EB2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EC2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="ED2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EE2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EF2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EG2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EH2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EI2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EJ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EK2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EL2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EM2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EN2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EO2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EP2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EQ2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="ER2" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="ES2">
-        <v>0</v>
-      </c>
-      <c r="ET2">
-        <v>0</v>
-      </c>
-      <c r="EU2">
-        <v>0</v>
-      </c>
-      <c r="EV2">
-        <v>0</v>
-      </c>
-      <c r="EW2">
-        <v>0</v>
-      </c>
-      <c r="EX2">
-        <v>0</v>
-      </c>
-      <c r="EY2">
-        <v>0</v>
-      </c>
-      <c r="EZ2">
-        <v>0</v>
-      </c>
-      <c r="FA2">
-        <v>0</v>
-      </c>
-      <c r="FB2">
-        <v>0</v>
-      </c>
-      <c r="FC2">
-        <v>0</v>
-      </c>
-      <c r="FD2">
-        <v>0</v>
-      </c>
-      <c r="FE2">
-        <v>0</v>
-      </c>
-      <c r="FF2">
-        <v>0</v>
-      </c>
-      <c r="FG2">
-        <v>0</v>
-      </c>
-      <c r="FH2">
-        <v>0</v>
-      </c>
-      <c r="FI2">
-        <v>0</v>
-      </c>
-      <c r="FJ2">
-        <v>0</v>
-      </c>
-      <c r="FK2">
-        <v>0</v>
-      </c>
-      <c r="FL2">
-        <v>0</v>
-      </c>
-      <c r="FM2">
-        <v>0</v>
-      </c>
-      <c r="FN2">
-        <v>0</v>
-      </c>
-      <c r="FO2">
-        <v>0</v>
-      </c>
-      <c r="FP2">
-        <v>0</v>
-      </c>
-      <c r="FQ2">
-        <v>0</v>
-      </c>
-      <c r="FR2">
-        <v>0</v>
-      </c>
-      <c r="FS2">
-        <v>0</v>
-      </c>
-      <c r="FT2">
-        <v>0</v>
-      </c>
-      <c r="FU2">
-        <v>0</v>
-      </c>
-      <c r="FV2">
-        <v>0</v>
-      </c>
-      <c r="FW2">
-        <v>0</v>
-      </c>
-      <c r="FX2">
-        <v>0</v>
-      </c>
-      <c r="FY2">
-        <v>0</v>
-      </c>
-      <c r="FZ2">
-        <v>0</v>
-      </c>
-      <c r="GA2">
-        <v>0</v>
-      </c>
-      <c r="GB2">
-        <v>0</v>
-      </c>
-      <c r="GC2">
-        <v>0</v>
-      </c>
-      <c r="GD2">
-        <v>0</v>
-      </c>
-      <c r="GE2">
-        <v>0</v>
-      </c>
-      <c r="GF2">
-        <v>0</v>
-      </c>
-      <c r="GG2">
-        <v>0</v>
-      </c>
-      <c r="GH2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1">
-    <cfRule type="expression" dxfId="16" priority="68">
+    <cfRule type="expression" dxfId="1" priority="83">
       <formula>IF(ISNA(A1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AC1">
-    <cfRule type="expression" dxfId="15" priority="67">
+    <cfRule type="expression" dxfId="0" priority="82">
       <formula>IF(ISNA(X1),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>IF(ISNA(B2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:J2">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>IF(ISNA(F2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>IF(ISNA(K2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>IF(ISNA(M2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>IF(ISNA(N2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>IF(N2="Monaco",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>IF(N2="Xio",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>IF(N2="Pinnacle",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>IF(N2="Eclipse",TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>IF(ISNA(O2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:Q2">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>IF(ISNA(P2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:X2">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>IF(ISNA(S2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:AD2">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>IF(ISNA(Y2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:BP2">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF(ISNA(AE2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DC2:ER2">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(ISNA(DC2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
restore uploading data spreadsheet
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenziping/Desktop/20200918AAB/AABKoala/LocalProgram/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8909EF-08A8-AD4D-8A07-A67D1C09E435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DD9893-B188-B64C-971B-3185815558CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="35840" windowHeight="20600" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
+    <workbookView xWindow="4600" yWindow="3240" windowWidth="27440" windowHeight="16440" xr2:uid="{73A62333-CCB6-CA4C-8A8C-1227D78D8F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,156 +35,249 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>AuditID</t>
+  </si>
+  <si>
+    <t>RevisionNumber</t>
+  </si>
+  <si>
+    <t>FacilityName</t>
+  </si>
+  <si>
+    <t>FacilityID</t>
+  </si>
+  <si>
+    <t>Auditor1</t>
+  </si>
+  <si>
+    <t>Auditor2</t>
+  </si>
+  <si>
+    <t>Auditor3</t>
+  </si>
+  <si>
+    <t>AuditDate</t>
+  </si>
+  <si>
+    <t>RepDate</t>
+  </si>
+  <si>
+    <t>LinacModel</t>
+  </si>
+  <si>
+    <t>LinacManufacturer</t>
+  </si>
+  <si>
+    <t>PlanningSystemManufacturer</t>
+  </si>
+  <si>
+    <t>tps</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>kqFac</t>
+  </si>
+  <si>
+    <t>ACDS</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>fac_6</t>
+  </si>
+  <si>
+    <t>fac_10</t>
+  </si>
+  <si>
+    <t>fac_15</t>
+  </si>
+  <si>
+    <t>fac_18</t>
+  </si>
+  <si>
+    <t>fac_6FFF</t>
+  </si>
+  <si>
+    <t>fac_10FFF</t>
+  </si>
+  <si>
+    <t>TPR_6</t>
+  </si>
+  <si>
+    <t>TPR_10</t>
+  </si>
+  <si>
+    <t>TPR_15</t>
+  </si>
+  <si>
+    <t>TPR_18</t>
+  </si>
+  <si>
+    <t>TPR_6FFF</t>
+  </si>
+  <si>
+    <t>TPR_10FFF</t>
+  </si>
+  <si>
     <t>Reading_101106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_205106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_208106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_205206</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_208206</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_205306</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_208306</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_403106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_405106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_103110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_403110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_405110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_103115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_403115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_405115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_103118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_403118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_405118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_101105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_103109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_110109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_303109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reading_305109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Misdelivery_101106</t>
   </si>
   <si>
     <t>Misdelivery_110106</t>
@@ -298,269 +391,176 @@
     <t>Misdelivery_305109</t>
   </si>
   <si>
-    <t>Misdelivery_101106</t>
-  </si>
-  <si>
-    <t>TPR_6</t>
-  </si>
-  <si>
-    <t>TPR_10</t>
-  </si>
-  <si>
-    <t>TPR_15</t>
-  </si>
-  <si>
-    <t>TPR_18</t>
-  </si>
-  <si>
-    <t>TPR_6FFF</t>
-  </si>
-  <si>
-    <t>TPR_10FFF</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>AuditID</t>
-  </si>
-  <si>
-    <t>RevisionNumber</t>
-  </si>
-  <si>
-    <t>FacilityName</t>
-  </si>
-  <si>
-    <t>FacilityID</t>
-  </si>
-  <si>
-    <t>Auditor1</t>
-  </si>
-  <si>
-    <t>Auditor2</t>
-  </si>
-  <si>
-    <t>Auditor3</t>
-  </si>
-  <si>
-    <t>AuditDate</t>
-  </si>
-  <si>
-    <t>RepDate</t>
-  </si>
-  <si>
-    <t>LinacModel</t>
-  </si>
-  <si>
-    <t>LinacManufacturer</t>
-  </si>
-  <si>
-    <t>PlanningSystemManufacturer</t>
-  </si>
-  <si>
-    <t>tps</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>kqFac</t>
-  </si>
-  <si>
-    <t>ACDS</t>
-  </si>
-  <si>
-    <t>Phantom</t>
-  </si>
-  <si>
-    <t>fac_6</t>
-  </si>
-  <si>
-    <t>fac_10</t>
-  </si>
-  <si>
-    <t>fac_15</t>
-  </si>
-  <si>
-    <t>fac_18</t>
-  </si>
-  <si>
-    <t>fac_6FFF</t>
-  </si>
-  <si>
-    <t>fac_10FFF</t>
+    <t>c6_p11_6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p12_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p13_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p14_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p15_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p16_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p17_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p11_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p12_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p13_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p14_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p15_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p16_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p17_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p11_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p12_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p13_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p14_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p15_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p17_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p18_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p11_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p12_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p13_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p14_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p15_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p16_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c6_p17_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p11_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p12_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p13_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p14_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p15_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p16_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c7_p17_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p11_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p12_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p13_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p14_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p15_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p17_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>c8_p18_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p11_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>imrt_misdelivery_c6_p11_6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>imrt_misdelivery_c6_p12_6</t>
@@ -700,18 +700,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -755,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1083,472 +1083,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E457-5FC7-BA47-BE39-F879CFE5AF79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79CB4E9-1D64-AC4E-8AE1-99DCAA607CA3}">
   <dimension ref="A1:GH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="31" max="31" width="39.83203125" customWidth="1"/>
-    <col min="32" max="32" width="28.6640625" customWidth="1"/>
-    <col min="33" max="33" width="32.33203125" customWidth="1"/>
-    <col min="68" max="68" width="28.6640625" customWidth="1"/>
-    <col min="190" max="190" width="40.83203125" customWidth="1"/>
-    <col min="191" max="191" width="37.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:190" s="2" customFormat="1">
+    <row r="1" spans="1:190">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="CF1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="CG1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="CH1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="CI1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="CJ1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="CK1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="CL1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="CM1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="CN1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="CO1" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="CP1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="CQ1" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="CR1" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="CS1" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="CT1" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="CU1" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="CV1" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="CW1" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="CX1" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="CY1" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="CZ1" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="DA1" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="DB1" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>23</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>25</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>26</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>27</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>28</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>30</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>35</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>37</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>39</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>46</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>47</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>48</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>49</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>50</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>51</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>52</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>54</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>55</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>58</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>59</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>60</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>61</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>62</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>63</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>64</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>65</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>66</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>67</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>68</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>70</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>71</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>72</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>73</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>74</v>
-      </c>
       <c r="DC1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="ED1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="EE1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="EF1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="EH1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="EJ1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="EK1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="EL1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="EM1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="EN1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="EP1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="EQ1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="ER1" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="DD1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="DE1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="DF1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="DG1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="DH1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="DI1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="DJ1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="DK1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="DM1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="EA1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="EC1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="ED1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="EE1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="EF1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="EG1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="EH1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="EI1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="EK1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="EL1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="EM1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="EN1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="EO1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="EP1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="EQ1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="ER1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="ES1" s="2" t="s">
         <v>148</v>
@@ -1678,18 +1665,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1">
-    <cfRule type="expression" dxfId="1" priority="83">
+    <cfRule type="expression" dxfId="1" priority="311">
       <formula>IF(ISNA(A1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AC1">
-    <cfRule type="expression" dxfId="0" priority="82">
+    <cfRule type="expression" dxfId="0" priority="310">
       <formula>IF(ISNA(X1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resultRequest get Request complete
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmwan\Desktop\SD\LocalProgram\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E0A5C2-C921-4CFC-9801-736B3BE3622B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCB7CA-FD9D-444D-B164-E87031CF396C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1254" yWindow="3162" windowWidth="16062" windowHeight="8802" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
+    <workbookView xWindow="2772" yWindow="1398" windowWidth="16062" windowHeight="8802" xr2:uid="{58DCBAB4-1D87-6D4D-AB10-ABBF03993274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,17 +665,10 @@
     <t>African Palm Civet</t>
   </si>
   <si>
-    <t>FAC-028</t>
-  </si>
-  <si>
     <t>Velvet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Q4 2020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LinacModel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -727,10 +720,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sun</t>
-  </si>
-  <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>FAC-029</t>
+  </si>
+  <si>
+    <t>Q4 2021</t>
+  </si>
+  <si>
+    <t>Mon</t>
   </si>
 </sst>
 </file>
@@ -833,12 +832,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -1162,7 +1156,7 @@
   <dimension ref="A1:GH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
@@ -1194,7 +1188,7 @@
         <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>86</v>
@@ -1209,16 +1203,16 @@
         <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>91</v>
@@ -1227,16 +1221,16 @@
         <v>92</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>93</v>
@@ -1753,8 +1747,11 @@
       </c>
     </row>
     <row r="2" spans="1:190">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>1111</v>
+        <v>1284</v>
       </c>
       <c r="C2" s="6">
         <v>1111</v>
@@ -1763,37 +1760,37 @@
         <v>182</v>
       </c>
       <c r="E2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" t="s">
         <v>183</v>
       </c>
-      <c r="F2" t="s">
-        <v>184</v>
-      </c>
       <c r="I2" s="4">
-        <v>44076</v>
+        <v>44077</v>
       </c>
       <c r="J2" t="s">
+        <v>199</v>
+      </c>
+      <c r="K2" t="s">
         <v>185</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" t="s">
         <v>187</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O2" t="s">
         <v>188</v>
       </c>
-      <c r="M2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="O2" t="s">
-        <v>190</v>
-      </c>
       <c r="P2" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S2" s="5">
         <v>1.008</v>
@@ -1918,19 +1915,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1">
-    <cfRule type="expression" dxfId="2" priority="84">
+  <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1 D2">
+    <cfRule type="expression" dxfId="1" priority="84">
       <formula>IF(ISNA(A1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AC1">
-    <cfRule type="expression" dxfId="1" priority="83">
+    <cfRule type="expression" dxfId="0" priority="83">
       <formula>IF(ISNA(X1),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(ISNA(D2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
uploadingData.xlsx modified to new table name
</commit_message>
<xml_diff>
--- a/LocalProgram/upload/uploadingData.xlsx
+++ b/LocalProgram/upload/uploadingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmwan\Desktop\SD\LocalProgram\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcl/Desktop/AABKoala/LocalProgram/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAA9C7E-D037-4E29-AEC3-56E68C30F688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A97D37-9FCD-0743-90E4-F9E780D15682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2916" yWindow="1344" windowWidth="16062" windowHeight="8802" xr2:uid="{73A62333-CCB6-CA4C-8A8C-1227D78D8F69}"/>
+    <workbookView xWindow="2920" yWindow="1340" windowWidth="16060" windowHeight="8800" xr2:uid="{73A62333-CCB6-CA4C-8A8C-1227D78D8F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,158 +231,6 @@
     <t>TPR_10FFF</t>
   </si>
   <si>
-    <t>Reading_101106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_205106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_208106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_205206</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_208206</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_205306</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_208306</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_403106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_405106</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_103110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_403110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_405110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_103115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_403115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_405115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_103118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_403118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_405118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_101105</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110105</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303105</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305105</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_103109</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_110109</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_303109</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reading_305109</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Misdelivery_101106</t>
   </si>
   <si>
@@ -495,174 +343,6 @@
   </si>
   <si>
     <t>Misdelivery_305109</t>
-  </si>
-  <si>
-    <t>c6_p11_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p12_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p13_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p14_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p15_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p16_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p17_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p11_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p12_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p13_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p14_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p15_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p16_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p17_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p11_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p12_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p13_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p14_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p15_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p17_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p18_6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p11_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p12_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p13_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p14_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p15_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p16_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c6_p17_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p11_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p12_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p13_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p14_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p15_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p16_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c7_p17_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p11_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p12_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p13_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p14_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p15_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p17_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8_p18_10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>imrt_misdelivery_c6_p11_6</t>
@@ -889,6 +569,246 @@
   </si>
   <si>
     <t>Tiny</t>
+  </si>
+  <si>
+    <t>code_101106</t>
+  </si>
+  <si>
+    <t>code_110106</t>
+  </si>
+  <si>
+    <t>code_205106</t>
+  </si>
+  <si>
+    <t>code_208106</t>
+  </si>
+  <si>
+    <t>code_205206</t>
+  </si>
+  <si>
+    <t>code_208206</t>
+  </si>
+  <si>
+    <t>code_205306</t>
+  </si>
+  <si>
+    <t>code_208306</t>
+  </si>
+  <si>
+    <t>code_303106</t>
+  </si>
+  <si>
+    <t>code_305106</t>
+  </si>
+  <si>
+    <t>code_403106</t>
+  </si>
+  <si>
+    <t>code_405106</t>
+  </si>
+  <si>
+    <t>code_103110</t>
+  </si>
+  <si>
+    <t>code_110110</t>
+  </si>
+  <si>
+    <t>code_303110</t>
+  </si>
+  <si>
+    <t>code_305110</t>
+  </si>
+  <si>
+    <t>code_403110</t>
+  </si>
+  <si>
+    <t>code_405110</t>
+  </si>
+  <si>
+    <t>code_103115</t>
+  </si>
+  <si>
+    <t>code_110115</t>
+  </si>
+  <si>
+    <t>code_303115</t>
+  </si>
+  <si>
+    <t>code_305115</t>
+  </si>
+  <si>
+    <t>code_403115</t>
+  </si>
+  <si>
+    <t>code_405115</t>
+  </si>
+  <si>
+    <t>code_103118</t>
+  </si>
+  <si>
+    <t>code_110118</t>
+  </si>
+  <si>
+    <t>code_303118</t>
+  </si>
+  <si>
+    <t>code_305118</t>
+  </si>
+  <si>
+    <t>code_403118</t>
+  </si>
+  <si>
+    <t>code_405118</t>
+  </si>
+  <si>
+    <t>code_101105</t>
+  </si>
+  <si>
+    <t>code_110105</t>
+  </si>
+  <si>
+    <t>code_303105</t>
+  </si>
+  <si>
+    <t>code_305105</t>
+  </si>
+  <si>
+    <t>code_103109</t>
+  </si>
+  <si>
+    <t>code_110109</t>
+  </si>
+  <si>
+    <t>code_303109</t>
+  </si>
+  <si>
+    <t>code_305109</t>
+  </si>
+  <si>
+    <t>code_c6_p11_6</t>
+  </si>
+  <si>
+    <t>code_c6_p12_6</t>
+  </si>
+  <si>
+    <t>code_c6_p13_6</t>
+  </si>
+  <si>
+    <t>code_c6_p14_6</t>
+  </si>
+  <si>
+    <t>code_c6_p15_6</t>
+  </si>
+  <si>
+    <t>code_c6_p16_6</t>
+  </si>
+  <si>
+    <t>code_c6_p17_6</t>
+  </si>
+  <si>
+    <t>code_c7_p11_6</t>
+  </si>
+  <si>
+    <t>code_c7_p12_6</t>
+  </si>
+  <si>
+    <t>code_c7_p13_6</t>
+  </si>
+  <si>
+    <t>code_c7_p14_6</t>
+  </si>
+  <si>
+    <t>code_c7_p15_6</t>
+  </si>
+  <si>
+    <t>code_c7_p16_6</t>
+  </si>
+  <si>
+    <t>code_c7_p17_6</t>
+  </si>
+  <si>
+    <t>code_c8_p11_6</t>
+  </si>
+  <si>
+    <t>code_c8_p12_6</t>
+  </si>
+  <si>
+    <t>code_c8_p13_6</t>
+  </si>
+  <si>
+    <t>code_c8_p14_6</t>
+  </si>
+  <si>
+    <t>code_c8_p15_6</t>
+  </si>
+  <si>
+    <t>code_c8_p17_6</t>
+  </si>
+  <si>
+    <t>code_c8_p18_6</t>
+  </si>
+  <si>
+    <t>code_c6_p11_10</t>
+  </si>
+  <si>
+    <t>code_c6_p12_10</t>
+  </si>
+  <si>
+    <t>code_c6_p13_10</t>
+  </si>
+  <si>
+    <t>code_c6_p14_10</t>
+  </si>
+  <si>
+    <t>code_c6_p15_10</t>
+  </si>
+  <si>
+    <t>code_c6_p16_10</t>
+  </si>
+  <si>
+    <t>code_c6_p17_10</t>
+  </si>
+  <si>
+    <t>code_c7_p11_10</t>
+  </si>
+  <si>
+    <t>code_c7_p12_10</t>
+  </si>
+  <si>
+    <t>code_c7_p13_10</t>
+  </si>
+  <si>
+    <t>code_c7_p14_10</t>
+  </si>
+  <si>
+    <t>code_c7_p15_10</t>
+  </si>
+  <si>
+    <t>code_c7_p16_10</t>
+  </si>
+  <si>
+    <t>code_c7_p17_10</t>
+  </si>
+  <si>
+    <t>code_c8_p11_10</t>
+  </si>
+  <si>
+    <t>code_c8_p12_10</t>
+  </si>
+  <si>
+    <t>code_c8_p13_10</t>
+  </si>
+  <si>
+    <t>code_c8_p14_10</t>
+  </si>
+  <si>
+    <t>code_c8_p15_10</t>
+  </si>
+  <si>
+    <t>code_c8_p17_10</t>
+  </si>
+  <si>
+    <t>code_c8_p18_10</t>
   </si>
 </sst>
 </file>
@@ -896,16 +816,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="0.0%"/>
-    <numFmt numFmtId="178" formatCode="0.00000000000"/>
-    <numFmt numFmtId="179" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -919,7 +839,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -927,13 +847,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1012,26 +932,36 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -1153,7 +1083,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1451,11 +1381,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79CB4E9-1D64-AC4E-8AE1-99DCAA607CA3}">
   <dimension ref="A1:GH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="GD1" workbookViewId="0">
+      <selection activeCell="GI3" sqref="GI3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="190" max="190" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:190">
       <c r="A1" s="1" t="s">
@@ -1549,484 +1483,484 @@
         <v>29</v>
       </c>
       <c r="AE1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>164</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>165</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>166</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>167</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>170</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>171</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>173</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>174</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>175</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>176</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>178</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>179</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BR1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="BS1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="BT1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="BU1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="BV1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BW1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BX1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BY1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BZ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="CA1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="CB1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="CC1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="CD1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="CE1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="CF1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="CG1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="CH1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="CI1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="CJ1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="CK1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="CL1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="CM1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="CN1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="CO1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="CP1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="CQ1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="CR1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="CS1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="CT1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="CU1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="CV1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="CW1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="CX1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="CY1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="CZ1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="DA1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="DB1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="DC1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="DV1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="DW1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="DX1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="DY1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DZ1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="EB1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="ED1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="EE1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="EF1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="EH1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="EI1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EJ1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="EK1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="EL1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="EM1" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="EN1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="EP1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="EQ1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="ER1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="ES1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="ET1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="EU1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="EV1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="EW1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="EX1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="EY1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="EZ1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="FA1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="FB1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="FC1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="FD1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="FE1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="FF1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="FG1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="FH1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="FI1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="FJ1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="FK1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="FL1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="FM1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="FN1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="FO1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="FP1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="FQ1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="FR1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="FS1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="FT1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="FU1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="FV1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="FW1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="FX1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="FY1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="FZ1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="GA1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="GB1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="GC1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="GD1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="GE1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="GF1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="GG1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="GH1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="DG1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="DH1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="DI1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="DJ1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="DK1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="DM1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="EA1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="EC1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="ED1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="EE1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="EF1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="EG1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="EH1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="EJ1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="EK1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="EL1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="EM1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="EN1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="EO1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="EP1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="EQ1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="ER1" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="ES1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="ET1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="EU1" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="EV1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="EW1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="EX1" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="EY1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="EZ1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="FA1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="FB1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="FC1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="FD1" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="FE1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="FF1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="FG1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="FH1" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="FI1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="FJ1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="FK1" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="FL1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="FM1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="FN1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="FO1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="FP1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="FQ1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="FR1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="FS1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="FT1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="FU1" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="FV1" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="FW1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="FX1" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="FY1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="FZ1" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="GA1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="GB1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="GC1" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="GD1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="GE1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="GF1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="GG1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="GH1" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:190">
@@ -2035,14 +1969,14 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6">
@@ -2050,25 +1984,25 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>193</v>
+        <v>113</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>194</v>
+        <v>114</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>195</v>
+        <v>115</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>196</v>
+        <v>116</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="R2" s="3"/>
       <c r="S2" s="7">
@@ -2660,14 +2594,14 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>199</v>
+        <v>119</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="6">
@@ -2675,25 +2609,25 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>194</v>
+        <v>114</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="7">
@@ -3285,14 +3219,14 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>207</v>
+        <v>127</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="6">
@@ -3300,25 +3234,25 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>208</v>
+        <v>128</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>209</v>
+        <v>129</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>211</v>
+        <v>131</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>212</v>
+        <v>132</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="10">
@@ -3909,14 +3843,14 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>213</v>
+        <v>133</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="6">
@@ -3924,25 +3858,25 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>215</v>
+        <v>135</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>216</v>
+        <v>136</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="7">
@@ -4533,44 +4467,44 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
-        <v>217</v>
+        <v>137</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>218</v>
+        <v>138</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="6">
         <v>41107</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>221</v>
+        <v>141</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>216</v>
+        <v>136</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>211</v>
+        <v>131</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="R6" s="3"/>
       <c r="S6" s="7">
@@ -5157,91 +5091,91 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B2:E6">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>IF(ISNA(B2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:J6">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>IF(ISNA(F2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K6">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>IF(ISNA(K2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L6">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>IF(ISNA(L2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L6">
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>IF(L2="Elekta",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>IF(L2="Varian",TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M6">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>IF(ISNA(M2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N6">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>IF(ISNA(N2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N6">
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>IF(N2="Monaco",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>IF(N2="Xio",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>IF(N2="Pinnacle",TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11">
+      <formula>IF(N2="Eclipse",TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O6">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>IF(ISNA(O2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:R6">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>IF(ISNA(P2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:AD6">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>IF(ISNA(S2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2:BP6">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>IF(ISNA(AE2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DC2:ER6">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF(ISNA(DC2),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1 D1:E1 G1:W1">
-    <cfRule type="expression" dxfId="18" priority="328">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>IF(ISNA(A1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AC1">
-    <cfRule type="expression" dxfId="17" priority="327">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(ISNA(X1),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E6">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>IF(ISNA(B2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:J6">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>IF(ISNA(F2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K6">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>IF(ISNA(K2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L6">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>IF(ISNA(L2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L6">
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>IF(L2="Elekta",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>IF(L2="Varian",TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M6">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>IF(ISNA(M2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N6">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>IF(ISNA(N2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N6">
-    <cfRule type="expression" dxfId="8" priority="6">
-      <formula>IF(N2="Monaco",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>IF(N2="Xio",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>IF(N2="Pinnacle",TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
-      <formula>IF(N2="Eclipse",TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O6">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>IF(ISNA(O2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:R6">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>IF(ISNA(P2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:AD6">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>IF(ISNA(S2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:BP6">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF(ISNA(AE2),TRUE,FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DC2:ER6">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(ISNA(DC2),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>